<commit_message>
On and Off Switch implemented
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Tag</t>
   </si>
@@ -42,6 +42,9 @@
     <t>Day</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>Work</t>
   </si>
   <si>
@@ -57,6 +60,9 @@
     <t>PALE_GREEN</t>
   </si>
   <si>
+    <t>On</t>
+  </si>
+  <si>
     <t>Exercise</t>
   </si>
   <si>
@@ -67,6 +73,9 @@
   </si>
   <si>
     <t>PALE_BLUE</t>
+  </si>
+  <si>
+    <t>Off</t>
   </si>
   <si>
     <t>Chores</t>
@@ -107,7 +116,7 @@
     <numFmt numFmtId="164" formatCode="h:mm am/pm"/>
     <numFmt numFmtId="165" formatCode="h:mm:ss am/pm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.000000"/>
       <color theme="1"/>
@@ -118,6 +127,13 @@
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.000000"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
@@ -149,18 +165,19 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,7 +689,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -707,149 +724,167 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3">
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>0.6875</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.78125</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.22916666666666666</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.78125</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="4">
         <v>0.375</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>0.91666666666666663</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>26</v>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="5"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="13">
-      <c r="H13" s="2"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14">
-      <c r="H14" s="2"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15">
-      <c r="H15" s="2"/>
+      <c r="H15" s="3"/>
     </row>
     <row r="16">
-      <c r="H16" s="2"/>
+      <c r="H16" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -859,7 +894,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{005A00CA-00F3-400B-B8A2-009B007800BE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00630075-0045-4B7C-BD2B-00D400C90028}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>"PALE_BLUE,PALE_GREEN,MAUVE,PALE_RED,YELLOW,ORANGE,CYAN,GRAY,BLUE"</xm:f>
           </x14:formula1>

</xml_diff>